<commit_message>
comprehensively test all DynamicExpressions and DynamicComponent; eliminated handmade approximately equals test; add DynamicRateLaws and DynamicDfbaObjectives to DynamicModel
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_dynamic_expressions.xlsx
+++ b/tests/fixtures/test_dynamic_expressions.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="7480" windowWidth="31920" windowHeight="14120" tabRatio="993" firstSheet="8" activeTab="19"/>
-    <workbookView xWindow="-21200" yWindow="9220" windowWidth="20200" windowHeight="12120" tabRatio="500" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="4040" yWindow="7480" windowWidth="31920" windowHeight="14120" tabRatio="993" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="-22420" yWindow="9280" windowWidth="22140" windowHeight="12060" tabRatio="500" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -24,52 +24,50 @@
     <sheet name="!!Initial species concentration" sheetId="9" r:id="rId9"/>
     <sheet name="!!Observables" sheetId="10" r:id="rId10"/>
     <sheet name="!!Functions" sheetId="11" r:id="rId11"/>
-    <sheet name="Broken Functions" sheetId="25" r:id="rId12"/>
-    <sheet name="!!Reactions" sheetId="12" r:id="rId13"/>
-    <sheet name="!!Rate laws" sheetId="13" r:id="rId14"/>
-    <sheet name="broken Rate law" sheetId="26" r:id="rId15"/>
-    <sheet name="!!dFBA objectives" sheetId="14" r:id="rId16"/>
-    <sheet name="!!dFBA objective reactions" sheetId="15" r:id="rId17"/>
-    <sheet name="!!dFBA objective species" sheetId="16" r:id="rId18"/>
-    <sheet name="!!Parameters" sheetId="17" r:id="rId19"/>
-    <sheet name="!!Stop conditions" sheetId="18" r:id="rId20"/>
-    <sheet name="!!Observations" sheetId="19" r:id="rId21"/>
-    <sheet name="!!Observation sets" sheetId="20" r:id="rId22"/>
-    <sheet name="!!Conclusions" sheetId="21" r:id="rId23"/>
-    <sheet name="!!References" sheetId="22" r:id="rId24"/>
-    <sheet name="!!Authors" sheetId="23" r:id="rId25"/>
-    <sheet name="!!Changes" sheetId="24" r:id="rId26"/>
+    <sheet name="!!Reactions" sheetId="12" r:id="rId12"/>
+    <sheet name="!!Rate laws" sheetId="13" r:id="rId13"/>
+    <sheet name="!!dFBA objectives" sheetId="14" r:id="rId14"/>
+    <sheet name="!!dFBA objective reactions" sheetId="15" r:id="rId15"/>
+    <sheet name="!!dFBA objective species" sheetId="16" r:id="rId16"/>
+    <sheet name="!!Parameters" sheetId="17" r:id="rId17"/>
+    <sheet name="!!Stop conditions" sheetId="18" r:id="rId18"/>
+    <sheet name="!!Observations" sheetId="19" r:id="rId19"/>
+    <sheet name="!!Observation sets" sheetId="20" r:id="rId20"/>
+    <sheet name="!!Conclusions" sheetId="21" r:id="rId21"/>
+    <sheet name="!!References" sheetId="22" r:id="rId22"/>
+    <sheet name="!!Authors" sheetId="23" r:id="rId23"/>
+    <sheet name="!!Changes" sheetId="24" r:id="rId24"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId25"/>
+    <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
     <externalReference r:id="rId28"/>
     <externalReference r:id="rId29"/>
-    <externalReference r:id="rId30"/>
-    <externalReference r:id="rId31"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$1:$C$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'!!Compartments'!$A$2:$G$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'!!Reactions'!$A$2:$D$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'!!References'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'!!Reactions'!$A$2:$D$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'!!References'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!!Species types'!$A$2:$K$8</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="18">[2]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="12">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="23">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="18">[2]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="12">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="23">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="18">[2]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="12">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="23">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -82,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="352">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
   </si>
@@ -351,9 +349,6 @@
     <t>dimensionless</t>
   </si>
   <si>
-    <t>Simple volume for testing</t>
-  </si>
-  <si>
     <t>!!ObjTables Type='Data' Id='SpeciesType' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
@@ -789,12 +784,6 @@
     <t>Rate law 8</t>
   </si>
   <si>
-    <t>k_cat_8 * volume_comp</t>
-  </si>
-  <si>
-    <t>Uses Parameters</t>
-  </si>
-  <si>
     <t>!!ObjTables Type='Data' Id='DfbaObjective' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
@@ -1081,6 +1070,72 @@
   </si>
   <si>
     <t>Uses a 'Compartment', i.e., its mass; sum over species</t>
+  </si>
+  <si>
+    <t>stop_condition_1</t>
+  </si>
+  <si>
+    <t>stop_condition_2</t>
+  </si>
+  <si>
+    <t>stop_condition_3</t>
+  </si>
+  <si>
+    <t>stop_condition_4</t>
+  </si>
+  <si>
+    <t>stop_condition_5</t>
+  </si>
+  <si>
+    <t>stop_condition_6</t>
+  </si>
+  <si>
+    <t>stop_condition_7</t>
+  </si>
+  <si>
+    <t>0 &lt; 1</t>
+  </si>
+  <si>
+    <t>k_cat_7 == 3</t>
+  </si>
+  <si>
+    <t>k_cat_8 &lt;= species_1[comp]</t>
+  </si>
+  <si>
+    <t>observable_3 &lt; species_1[comp]</t>
+  </si>
+  <si>
+    <t>2 &lt;1</t>
+  </si>
+  <si>
+    <t>comp &lt; k_cat_9</t>
+  </si>
+  <si>
+    <t>Simple volume for testing; expression for compartment evaluates to its mass</t>
+  </si>
+  <si>
+    <t>Uses a Function</t>
+  </si>
+  <si>
+    <t>0.4 &lt; function_6 &lt;= 10</t>
+  </si>
+  <si>
+    <t>Uses a 'Compartment', i.e., its mass</t>
+  </si>
+  <si>
+    <t>k_cat_10 * volume_comp</t>
+  </si>
+  <si>
+    <t>liter^-1 s^-1</t>
+  </si>
+  <si>
+    <t>Uses Parameters and compartment volume function</t>
+  </si>
+  <si>
+    <t>Linear function of species</t>
+  </si>
+  <si>
+    <t>Expression of other observable and species</t>
   </si>
 </sst>
 </file>
@@ -1191,15 +1246,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1276,6 +1333,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1294,17 +1358,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1924,8 +1998,8 @@
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomRight" activeCell="H3" sqref="H3:H9"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="H2" sqref="H2:K2"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1934,9 +2008,9 @@
     <col min="2" max="2" width="8.83203125" style="17" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="17" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="17" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="17" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="17" customWidth="1"/>
     <col min="10" max="10" width="29.6640625" style="17" bestFit="1" customWidth="1"/>
@@ -1948,7 +2022,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1959,7 +2033,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>79</v>
@@ -1980,21 +2054,21 @@
         <v>54</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H3" s="24">
         <v>1000000000</v>
@@ -2006,13 +2080,13 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H4" s="24">
         <v>2000000000</v>
@@ -2024,13 +2098,13 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H5" s="24">
         <v>3000000000</v>
@@ -2042,49 +2116,52 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H6" s="17">
         <v>481771260.80000001</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="28">
         <f>'!!Initial species concentration'!E6*'!!Compartments'!I4*'!!Parameters'!D14</f>
         <v>481771260.80000001</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>144</v>
-      </c>
       <c r="D7" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H7" s="17">
         <v>1083985336.8</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="28">
         <f>J6 + '!!Initial species concentration'!E7*'!!Compartments'!I4*'!!Parameters'!D14</f>
         <v>1083985336.8</v>
       </c>
+      <c r="K7" s="17" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>146</v>
-      </c>
       <c r="D8" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H8" s="17">
         <v>4000000000</v>
@@ -2096,20 +2173,23 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>148</v>
-      </c>
       <c r="D9" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H9" s="17">
         <v>1083985336.8</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="28">
         <f>J6 + '!!Initial species concentration'!E7*'!!Compartments'!I4*'!!Parameters'!D14</f>
         <v>1083985336.8</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -2120,32 +2200,32 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2:K2"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <selection activeCell="A13" sqref="A13:XFD17"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="1">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="22" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" style="22" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="22" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="22" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="26.83203125" style="22" customWidth="1"/>
-    <col min="11" max="11" width="50.6640625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="14" style="22" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="22" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" style="22" customWidth="1"/>
+    <col min="11" max="11" width="46.83203125" style="22" customWidth="1"/>
     <col min="12" max="12" width="12.5" style="22" customWidth="1"/>
     <col min="13" max="1026" width="8.83203125" style="22" customWidth="1"/>
     <col min="1027" max="1028" width="9" style="22" customWidth="1"/>
@@ -2154,7 +2234,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -2165,7 +2245,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>79</v>
@@ -2186,17 +2266,17 @@
         <v>54</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
+        <v>328</v>
+      </c>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="22">
         <v>0.1</v>
@@ -2207,17 +2287,17 @@
       <c r="H3" s="22">
         <v>0.1</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="36">
         <f>0.1</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>151</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>152</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>88</v>
@@ -2225,80 +2305,80 @@
       <c r="H4" s="22">
         <v>0.5</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="36">
         <f>0.5 / EXP(0)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>87</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H5" s="22">
         <v>1100</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="36">
         <f>'!!Parameters'!D15</f>
         <v>1100</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>156</v>
-      </c>
       <c r="D6" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H6" s="22">
         <v>3000000000</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="36">
         <f>'!!Initial species concentration'!E3 + '!!Initial species concentration'!E4</f>
         <v>3000000000</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H7" s="22">
         <v>3000000000</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="36">
         <f>'!!Observables'!J5</f>
         <v>3000000000</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>160</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>161</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>88</v>
@@ -2306,56 +2386,106 @@
       <c r="H8" s="22">
         <v>0.6</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="36">
         <f>J3+J4</f>
         <v>0.6</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>81</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H9" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="37">
         <f>'!!Compartments'!V4</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>168</v>
-      </c>
       <c r="D10" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H10" s="22">
         <v>2000000000</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="36">
         <f>'!!Observables'!J5 - J7 + '!!Initial species concentration'!E4</f>
         <v>2000000000</v>
       </c>
       <c r="K10" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
         <v>169</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="22">
+        <v>2E-3</v>
+      </c>
+      <c r="J11" s="37">
+        <f>'!!Compartments'!V4 / '!!Parameters'!D15</f>
+        <v>2E-3</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>320</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J12" s="37">
+        <f xml:space="preserve"> '!!Parameters'!D15 * J11+ '!!Compartments'!V4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2365,102 +2495,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="M17" sqref="M17"/>
-      <selection pane="topRight" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.83203125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="26" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="26" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="48.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="1026" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1027" max="1028" width="9" style="26" customWidth="1"/>
-    <col min="1029" max="16384" width="9" style="26"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>324</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>166</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
@@ -2494,7 +2528,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2504,11 +2538,11 @@
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="G2" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -2523,22 +2557,22 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>179</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>180</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>79</v>
@@ -2559,49 +2593,49 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>181</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>182</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E4" s="22">
         <v>0</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="25"/>
       <c r="M4" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>185</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>186</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E5" s="22">
         <v>0</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -2610,167 +2644,167 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>187</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>188</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E6" s="14">
         <v>0</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>189</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>190</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E7" s="22">
         <v>0</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>191</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>192</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E8" s="22">
         <v>0</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>193</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>194</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E9" s="22">
         <v>0</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>195</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>196</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E10" s="22">
         <v>0</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>197</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>198</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E11" s="22">
         <v>0</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>199</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>200</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E12" s="22">
         <v>0</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>201</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>202</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E13" s="22">
         <v>0</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2783,18 +2817,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2:N2"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="1">
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="1">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -2803,12 +2837,13 @@
     <col min="1" max="1" width="19" style="22" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="22" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="43.83203125" style="22" customWidth="1"/>
     <col min="7" max="7" width="9.1640625" style="22" customWidth="1"/>
     <col min="8" max="10" width="9.1640625" style="22" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="22" customWidth="1"/>
-    <col min="12" max="13" width="8.83203125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" style="38" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="22" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="38" customWidth="1"/>
     <col min="14" max="14" width="52.1640625" style="22" customWidth="1"/>
     <col min="15" max="1025" width="8.83203125" style="22" customWidth="1"/>
     <col min="1026" max="1027" width="9" style="22" customWidth="1"/>
@@ -2817,10 +2852,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="70" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="27" customFormat="1" ht="70" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -2828,16 +2863,16 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>205</v>
-      </c>
       <c r="E2" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>79</v>
@@ -2858,220 +2893,254 @@
         <v>54</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>208</v>
-      </c>
       <c r="F3" s="26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="K3" s="22">
+        <v>182</v>
+      </c>
+      <c r="K3" s="38">
         <v>1</v>
       </c>
-      <c r="M3" s="22">
+      <c r="M3" s="38">
         <f>'!!Parameters'!J4</f>
         <v>1</v>
       </c>
       <c r="N3" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>211</v>
-      </c>
       <c r="G4" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="K4" s="22">
+        <v>182</v>
+      </c>
+      <c r="K4" s="38">
         <v>0.2</v>
       </c>
-      <c r="M4" s="22">
+      <c r="M4" s="38">
         <f>'!!Parameters'!J5/10</f>
         <v>0.2</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>215</v>
-      </c>
       <c r="G5" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="K5" s="22">
+        <v>182</v>
+      </c>
+      <c r="K5" s="38">
         <v>3000000000</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="38">
         <f>'!!Parameters'!J6 * '!!Initial species concentration'!E3</f>
         <v>3000000000</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="C6" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>219</v>
-      </c>
       <c r="G6" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="K6" s="22">
+        <v>182</v>
+      </c>
+      <c r="K6" s="38">
         <v>1927085043.2</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="39">
         <f>'!!Parameters'!J7 * '!!Observables'!J6</f>
         <v>1927085043.2</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="C7" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F7" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>223</v>
-      </c>
       <c r="G7" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="K7" s="22">
+        <v>182</v>
+      </c>
+      <c r="K7" s="38">
         <v>600000000</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="39">
         <f>'!!Functions'!J6 / '!!Parameters'!J8</f>
         <v>600000000</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="C8" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>227</v>
-      </c>
       <c r="G8" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="K8" s="22">
+        <v>182</v>
+      </c>
+      <c r="K8" s="38">
         <v>13.200000000000001</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="39">
         <f>'!!Parameters'!J9 * '!!Compartments'!V4</f>
         <v>13.200000000000001</v>
       </c>
       <c r="N8" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="C9" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>231</v>
-      </c>
       <c r="G9" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="K9" s="22">
+        <v>182</v>
+      </c>
+      <c r="K9" s="38">
         <v>5527085056.3999996</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="39">
         <f>M5 + M6 + M7 + M8</f>
         <v>5527085056.3999996</v>
       </c>
       <c r="N9" s="22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
         <v>232</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="M10" s="39">
+        <f>'!!Parameters'!D13 * '!!Functions'!J11</f>
+        <v>0.02</v>
+      </c>
+      <c r="N10" s="27" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -3080,107 +3149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="M17" sqref="M17"/>
-      <selection pane="topRight" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A3:XFD9"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19" style="26" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="43.83203125" style="26" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="26" customWidth="1"/>
-    <col min="8" max="10" width="9.1640625" style="26" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="36.6640625" style="26" customWidth="1"/>
-    <col min="12" max="1025" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1026" max="1027" width="9" style="26" customWidth="1"/>
-    <col min="1028" max="16384" width="9" style="26"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>236</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -3205,7 +3174,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -3216,19 +3185,19 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>79</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>44</v>
@@ -3248,19 +3217,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>88</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>43</v>
@@ -3271,7 +3240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -3298,7 +3267,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3309,13 +3278,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>79</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>44</v>
@@ -3335,22 +3304,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>243</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3359,7 +3328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -3388,7 +3357,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -3399,13 +3368,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>79</v>
@@ -3428,45 +3397,45 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="10">
         <v>-3</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3475,7 +3444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
@@ -3484,10 +3453,10 @@
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3499,7 +3468,7 @@
     <col min="6" max="6" width="24.33203125" style="22" customWidth="1"/>
     <col min="7" max="9" width="8.83203125" style="22" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="6" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21.83203125" style="6" customWidth="1"/>
     <col min="13" max="13" width="46.5" style="6" customWidth="1"/>
     <col min="14" max="1026" width="8.83203125" style="6" customWidth="1"/>
@@ -3509,7 +3478,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
@@ -3520,13 +3489,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>79</v>
@@ -3547,18 +3516,18 @@
         <v>54</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D3" s="22">
         <v>0.3</v>
@@ -3570,16 +3539,16 @@
         <v>0.3</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D4" s="26">
         <v>1</v>
@@ -3588,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
@@ -3600,10 +3569,10 @@
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="22" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D5" s="22">
         <v>2</v>
@@ -3612,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J5" s="26">
         <v>2</v>
@@ -3620,10 +3589,10 @@
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D6" s="22">
         <v>3</v>
@@ -3632,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J6" s="26">
         <v>3</v>
@@ -3640,10 +3609,10 @@
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D7" s="22">
         <v>4</v>
@@ -3652,7 +3621,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J7" s="26">
         <v>4</v>
@@ -3660,10 +3629,10 @@
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="22" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D8" s="22">
         <v>5</v>
@@ -3672,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J8" s="26">
         <v>5</v>
@@ -3680,10 +3649,10 @@
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D9" s="22">
         <v>6</v>
@@ -3692,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="J9" s="26">
         <v>6</v>
@@ -3700,10 +3669,10 @@
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D10" s="22">
         <v>7</v>
@@ -3711,50 +3680,59 @@
       <c r="E10" s="22">
         <v>0</v>
       </c>
+      <c r="F10" s="22" t="s">
+        <v>88</v>
+      </c>
       <c r="J10" s="26">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="22" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>256</v>
-      </c>
-      <c r="D11" s="22">
-        <v>8</v>
+        <v>253</v>
+      </c>
+      <c r="D11" s="27">
+        <v>1000000000</v>
       </c>
       <c r="E11" s="22">
         <v>0</v>
       </c>
-      <c r="J11" s="26">
-        <v>8</v>
+      <c r="F11" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" s="27">
+        <v>1000000000</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D12" s="22">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E12" s="22">
         <v>0</v>
       </c>
-      <c r="J12" s="26">
-        <v>9</v>
+      <c r="F12" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="J12" s="27">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="22" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D13" s="22">
         <v>10</v>
@@ -3762,13 +3740,16 @@
       <c r="E13" s="22">
         <v>0</v>
       </c>
-      <c r="J13" s="26">
+      <c r="F13" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="J13" s="27">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="22" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D14" s="7">
         <v>6.0221407599999999E+23</v>
@@ -3777,13 +3758,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J14" s="7">
         <v>6.0221407599999999E+23</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3797,13 +3778,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="J15" s="26">
         <v>1100</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3879,6 +3860,385 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M16" sqref="M16"/>
+      <selection pane="topRight" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" style="22" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="22" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="22" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="22" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="22" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="33" style="22" customWidth="1"/>
+    <col min="12" max="1026" width="8.83203125" style="22" customWidth="1"/>
+    <col min="1027" max="1028" width="9" style="22" customWidth="1"/>
+    <col min="1029" max="16384" width="9" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="26" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27" t="b">
+        <f>IF(0 &lt; 1, TRUE())</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="27"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27" t="b">
+        <f>IF(2 &lt;  1, TRUE())</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="27" t="b">
+        <f>IF('!!Parameters'!D10=3, TRUE())</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27" t="b">
+        <f>IF( '!!Parameters'!D11 &lt;= '!!Initial species concentration'!E3, TRUE())</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27" t="b">
+        <f>IF( '!!Observables'!H5 &lt;= '!!Initial species concentration'!E3, TRUE())</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27" t="b">
+        <f>IF( AND(0.4 &lt; '!!Functions'!J8,  '!!Functions'!J8 &lt;= 10), TRUE())</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27" t="b">
+        <f>IF( '!!Compartments'!V4 &lt; '!!Parameters'!D12, TRUE())</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M16" sqref="M16"/>
+      <selection pane="topRight" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9" style="22" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="G2" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="Q2" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="R2" s="31"/>
+      <c r="S2" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="T2" s="31"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -4002,209 +4362,6 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="M16" sqref="M16"/>
-      <selection pane="topRight" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="8.83203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="22" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="22" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="8.83203125" style="22" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="22" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="22" customWidth="1"/>
-    <col min="11" max="11" width="33" style="22" customWidth="1"/>
-    <col min="12" max="1026" width="8.83203125" style="22" customWidth="1"/>
-    <col min="1027" max="1028" width="9" style="22" customWidth="1"/>
-    <col min="1029" max="16384" width="9" style="22"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="26" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>331</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W3"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="M16" sqref="M16"/>
-      <selection pane="topRight" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="9" style="22" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="22"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G2" s="31" t="s">
-        <v>272</v>
-      </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="Q2" s="32" t="s">
-        <v>274</v>
-      </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="32" t="s">
-        <v>275</v>
-      </c>
-      <c r="T2" s="28"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
@@ -4226,7 +4383,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4237,7 +4394,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>44</v>
@@ -4266,7 +4423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
@@ -4289,14 +4446,14 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="32" t="s">
-        <v>286</v>
-      </c>
-      <c r="H2" s="28"/>
+      <c r="G2" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -4306,16 +4463,16 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>31</v>
@@ -4336,10 +4493,10 @@
         <v>54</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4387,7 +4544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -4410,7 +4567,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4421,46 +4578,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="G2" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="N2" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="O2" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="P2" s="18" t="s">
         <v>299</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>302</v>
       </c>
       <c r="Q2" s="18" t="s">
         <v>44</v>
@@ -4476,7 +4633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -4497,7 +4654,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -4508,28 +4665,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>304</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>306</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>307</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>309</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>310</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4543,7 +4700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -4563,7 +4720,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -4574,28 +4731,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>315</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>318</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4613,10 +4770,10 @@
         <v>54</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -4863,7 +5020,7 @@
       <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
     </sheetView>
     <sheetView topLeftCell="F1" workbookViewId="1">
-      <selection activeCell="Y16" sqref="Y16"/>
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4877,10 +5034,10 @@
     <col min="8" max="16" width="8.83203125" style="22" customWidth="1"/>
     <col min="17" max="18" width="8.83203125" style="22" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="8.83203125" style="22" customWidth="1"/>
-    <col min="20" max="20" width="16.33203125" style="22" customWidth="1"/>
+    <col min="20" max="20" width="12.5" style="22" customWidth="1"/>
     <col min="21" max="21" width="8.83203125" style="22" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="8.83203125" style="22" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" style="22" customWidth="1"/>
+    <col min="23" max="23" width="33.1640625" style="22" customWidth="1"/>
     <col min="24" max="1035" width="8.83203125" style="22" customWidth="1"/>
     <col min="1036" max="1037" width="9" style="22" customWidth="1"/>
     <col min="1038" max="16384" width="9" style="22"/>
@@ -4899,19 +5056,19 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -5994,10 +6151,10 @@
         <v>54</v>
       </c>
       <c r="V3" s="18" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
@@ -7026,7 +7183,7 @@
         <v>85</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H4" s="22" t="s">
         <v>86</v>
@@ -7038,7 +7195,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="L4" s="22" t="s">
         <v>87</v>
@@ -7063,7 +7220,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="W4" s="22" t="s">
-        <v>89</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -7110,18 +7267,18 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C2" s="30" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
@@ -7131,25 +7288,25 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>44</v>
@@ -7169,10 +7326,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>100</v>
       </c>
       <c r="G4" s="22">
         <v>1</v>
@@ -7181,16 +7338,16 @@
         <v>0</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>102</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>103</v>
       </c>
       <c r="G5" s="22">
         <v>2</v>
@@ -7199,16 +7356,16 @@
         <v>0</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>105</v>
       </c>
       <c r="G6" s="22">
         <v>3</v>
@@ -7217,16 +7374,16 @@
         <v>0</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>106</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>107</v>
       </c>
       <c r="G7" s="22">
         <v>4</v>
@@ -7235,16 +7392,16 @@
         <v>0</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>109</v>
       </c>
       <c r="G8" s="22">
         <v>5</v>
@@ -7253,16 +7410,16 @@
         <v>0</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>110</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>111</v>
       </c>
       <c r="G9" s="22">
         <v>6</v>
@@ -7271,7 +7428,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -7318,7 +7475,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -7329,10 +7486,10 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>114</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>79</v>
@@ -7355,104 +7512,104 @@
     </row>
     <row r="3" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>116</v>
-      </c>
       <c r="C3" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>81</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>119</v>
-      </c>
       <c r="C4" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>81</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>121</v>
-      </c>
       <c r="C5" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>81</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>123</v>
-      </c>
       <c r="C6" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>126</v>
-      </c>
       <c r="C7" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>81</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>128</v>
-      </c>
       <c r="C8" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -7477,7 +7634,7 @@
       <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7500,7 +7657,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -7511,7 +7668,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>76</v>
@@ -7543,10 +7700,10 @@
     </row>
     <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>86</v>
@@ -7558,15 +7715,15 @@
         <v>0</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>86</v>
@@ -7578,15 +7735,15 @@
         <v>0</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>86</v>
@@ -7598,15 +7755,15 @@
         <v>0</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>86</v>
@@ -7618,15 +7775,15 @@
         <v>0</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>86</v>
@@ -7638,15 +7795,15 @@
         <v>0</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>86</v>
@@ -7658,7 +7815,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>